<commit_message>
Added CSV and updated graphs
</commit_message>
<xml_diff>
--- a/PV-Realisierte-Erzeugung-2024-daily.xlsx
+++ b/PV-Realisierte-Erzeugung-2024-daily.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Privat\Studium\HAW\4. Semester\IPJ2\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03EBDF2C-D9D0-48A3-B42A-D013C052CDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79AB39-46C4-491B-BD4C-83A1BFEB4D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2CA0663-2C25-422E-B284-C218A5CDAACD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{86D493EA-209B-4542-9EA0-9BCE29FFE870}"/>
   </bookViews>
   <sheets>
-    <sheet name="PV-Realisierte-Erzeugung-2024-d" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Datum von</t>
+    <t>Wert in MWh</t>
   </si>
   <si>
-    <t>Photovoltaik [MWh] Berechnete Auflösungen</t>
+    <t>Tage</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -887,2947 +887,2941 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{198BD505-9121-4E27-BEE8-D8000E952220}">
-  <dimension ref="A1:B367"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E8C282-A628-4C1E-8B70-9C01E93EEB21}">
+  <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>45292</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>38018</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>45293</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>10702.25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>45294</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>32264.75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>45295</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
         <v>26356.75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
         <v>25621</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>45297</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
         <v>13241.5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>45298</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>16333.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>45299</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
         <v>41129.25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>45300</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
         <v>75589.75</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>45301</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
         <v>70612</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>45302</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
         <v>65201</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>45303</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
         <v>21011.5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>45304</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
         <v>13296.5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>45305</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
         <v>34536.75</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>45306</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
         <v>22651.5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>45307</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
         <v>33751.75</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>45308</v>
-      </c>
-      <c r="B18" s="2">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
         <v>14472</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>45309</v>
-      </c>
-      <c r="B19" s="2">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
         <v>23482.75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>45310</v>
-      </c>
-      <c r="B20" s="2">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
         <v>32442.5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>45311</v>
-      </c>
-      <c r="B21" s="2">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
         <v>61247.75</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>45312</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
         <v>43170.25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>45313</v>
-      </c>
-      <c r="B23" s="2">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
         <v>22913</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>45314</v>
-      </c>
-      <c r="B24" s="2">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
         <v>54288.25</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>45315</v>
-      </c>
-      <c r="B25" s="2">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
         <v>40377</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>45316</v>
-      </c>
-      <c r="B26" s="2">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
         <v>65498.75</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>45317</v>
-      </c>
-      <c r="B27" s="2">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
         <v>24737.25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>45318</v>
-      </c>
-      <c r="B28" s="2">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
         <v>123524.25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>45319</v>
-      </c>
-      <c r="B29" s="2">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
         <v>142216.25</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>45320</v>
-      </c>
-      <c r="B30" s="2">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
         <v>124073</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>45321</v>
-      </c>
-      <c r="B31" s="2">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
         <v>76415.5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>45322</v>
-      </c>
-      <c r="B32" s="2">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
         <v>44627.75</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>45323</v>
-      </c>
-      <c r="B33" s="2">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
         <v>67201.5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>45324</v>
-      </c>
-      <c r="B34" s="2">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
         <v>48930.25</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>45325</v>
-      </c>
-      <c r="B35" s="2">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
         <v>51887.25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>45326</v>
-      </c>
-      <c r="B36" s="2">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
         <v>35799</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>45327</v>
-      </c>
-      <c r="B37" s="2">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
         <v>82874.5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>45328</v>
-      </c>
-      <c r="B38" s="2">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
         <v>44833.5</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>45329</v>
-      </c>
-      <c r="B39" s="2">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
         <v>45611.75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>45330</v>
-      </c>
-      <c r="B40" s="2">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
         <v>39536.75</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>45331</v>
-      </c>
-      <c r="B41" s="2">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
         <v>37277.75</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>45332</v>
-      </c>
-      <c r="B42" s="2">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
         <v>70696.25</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>45333</v>
-      </c>
-      <c r="B43" s="2">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
         <v>30264.25</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>45334</v>
-      </c>
-      <c r="B44" s="2">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
         <v>53982.5</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>45335</v>
-      </c>
-      <c r="B45" s="2">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
         <v>120545.25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>45336</v>
-      </c>
-      <c r="B46" s="2">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
         <v>53021.5</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>45337</v>
-      </c>
-      <c r="B47" s="2">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
         <v>86343.25</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>45338</v>
-      </c>
-      <c r="B48" s="2">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
         <v>85237</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>45339</v>
-      </c>
-      <c r="B49" s="2">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
         <v>80149.25</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>45340</v>
-      </c>
-      <c r="B50" s="2">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
         <v>90326.5</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>45341</v>
-      </c>
-      <c r="B51" s="2">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
         <v>55619</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
-        <v>45342</v>
-      </c>
-      <c r="B52" s="2">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
         <v>88504.25</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
-        <v>45343</v>
-      </c>
-      <c r="B53" s="2">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1">
         <v>106293.5</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>45344</v>
-      </c>
-      <c r="B54" s="2">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1">
         <v>43666</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>45345</v>
-      </c>
-      <c r="B55" s="2">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
         <v>84458.5</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>45346</v>
-      </c>
-      <c r="B56" s="2">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
         <v>141314</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
-        <v>45347</v>
-      </c>
-      <c r="B57" s="2">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
         <v>154637.5</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>45348</v>
-      </c>
-      <c r="B58" s="2">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
         <v>100958.75</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>45349</v>
-      </c>
-      <c r="B59" s="2">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
         <v>79709.75</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>45350</v>
-      </c>
-      <c r="B60" s="2">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
         <v>100875.25</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>45351</v>
-      </c>
-      <c r="B61" s="2">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
         <v>156351.25</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>45352</v>
-      </c>
-      <c r="B62" s="2">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
         <v>92550.25</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>45353</v>
-      </c>
-      <c r="B63" s="2">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
         <v>164759.5</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>45354</v>
-      </c>
-      <c r="B64" s="2">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
         <v>185383.25</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>45355</v>
-      </c>
-      <c r="B65" s="2">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1">
         <v>93207.25</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>45356</v>
-      </c>
-      <c r="B66" s="2">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1">
         <v>67234.25</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
-        <v>45357</v>
-      </c>
-      <c r="B67" s="2">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1">
         <v>114284.25</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
-        <v>45358</v>
-      </c>
-      <c r="B68" s="2">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
         <v>131133.5</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
-        <v>45359</v>
-      </c>
-      <c r="B69" s="2">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1">
         <v>247356</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
-        <v>45360</v>
-      </c>
-      <c r="B70" s="2">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1">
         <v>228277.75</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
-        <v>45361</v>
-      </c>
-      <c r="B71" s="2">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1">
         <v>135100.75</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
-        <v>45362</v>
-      </c>
-      <c r="B72" s="2">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1">
         <v>150435</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
-        <v>45363</v>
-      </c>
-      <c r="B73" s="2">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1">
         <v>84734</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
-        <v>45364</v>
-      </c>
-      <c r="B74" s="2">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1">
         <v>111560.25</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
-        <v>45365</v>
-      </c>
-      <c r="B75" s="2">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1">
         <v>172493</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
-        <v>45366</v>
-      </c>
-      <c r="B76" s="2">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1">
         <v>153149.5</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
-        <v>45367</v>
-      </c>
-      <c r="B77" s="2">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1">
         <v>120067.25</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
-        <v>45368</v>
-      </c>
-      <c r="B78" s="2">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1">
         <v>203607.75</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
-        <v>45369</v>
-      </c>
-      <c r="B79" s="2">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1">
         <v>148395.25</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
-        <v>45370</v>
-      </c>
-      <c r="B80" s="2">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1">
         <v>208684.75</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
-        <v>45371</v>
-      </c>
-      <c r="B81" s="2">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1">
         <v>220275.5</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
-        <v>45372</v>
-      </c>
-      <c r="B82" s="2">
+      <c r="A82" s="2">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1">
         <v>139776.5</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1">
-        <v>45373</v>
-      </c>
-      <c r="B83" s="2">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1">
         <v>141444.75</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
-        <v>45374</v>
-      </c>
-      <c r="B84" s="2">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1">
         <v>144938</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1">
-        <v>45375</v>
-      </c>
-      <c r="B85" s="2">
+      <c r="A85" s="2">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1">
         <v>122569.25</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="1">
-        <v>45376</v>
-      </c>
-      <c r="B86" s="2">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1">
         <v>223314</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="1">
-        <v>45377</v>
-      </c>
-      <c r="B87" s="2">
+      <c r="A87" s="2">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1">
         <v>226181.5</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
-        <v>45378</v>
-      </c>
-      <c r="B88" s="2">
+      <c r="A88" s="2">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1">
         <v>184237.75</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
-        <v>45379</v>
-      </c>
-      <c r="B89" s="2">
+      <c r="A89" s="2">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1">
         <v>151639</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="1">
-        <v>45380</v>
-      </c>
-      <c r="B90" s="2">
+      <c r="A90" s="2">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1">
         <v>137197</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="1">
-        <v>45381</v>
-      </c>
-      <c r="B91" s="2">
+      <c r="A91" s="2">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1">
         <v>165992.5</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="1">
-        <v>45382</v>
-      </c>
-      <c r="B92" s="2">
+      <c r="A92" s="2">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1">
         <v>206778</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="1">
-        <v>45383</v>
-      </c>
-      <c r="B93" s="2">
+      <c r="A93" s="2">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1">
         <v>89289.5</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="1">
-        <v>45384</v>
-      </c>
-      <c r="B94" s="2">
+      <c r="A94" s="2">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1">
         <v>179558.5</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="1">
-        <v>45385</v>
-      </c>
-      <c r="B95" s="2">
+      <c r="A95" s="2">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1">
         <v>118775.25</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="1">
-        <v>45386</v>
-      </c>
-      <c r="B96" s="2">
+      <c r="A96" s="2">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1">
         <v>127439</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="1">
-        <v>45387</v>
-      </c>
-      <c r="B97" s="2">
+      <c r="A97" s="2">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1">
         <v>194067.75</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="1">
-        <v>45388</v>
-      </c>
-      <c r="B98" s="2">
+      <c r="A98" s="2">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1">
         <v>290608</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="1">
-        <v>45389</v>
-      </c>
-      <c r="B99" s="2">
+      <c r="A99" s="2">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1">
         <v>235187</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="1">
-        <v>45390</v>
-      </c>
-      <c r="B100" s="2">
+      <c r="A100" s="2">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1">
         <v>250281.25</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="1">
-        <v>45391</v>
-      </c>
-      <c r="B101" s="2">
+      <c r="A101" s="2">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1">
         <v>147705.75</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="1">
-        <v>45392</v>
-      </c>
-      <c r="B102" s="2">
+      <c r="A102" s="2">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1">
         <v>209252.25</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="1">
-        <v>45393</v>
-      </c>
-      <c r="B103" s="2">
+      <c r="A103" s="2">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1">
         <v>242582.75</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="1">
-        <v>45394</v>
-      </c>
-      <c r="B104" s="2">
+      <c r="A104" s="2">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1">
         <v>254527.5</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="1">
-        <v>45395</v>
-      </c>
-      <c r="B105" s="2">
+      <c r="A105" s="2">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1">
         <v>291841.25</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="1">
-        <v>45396</v>
-      </c>
-      <c r="B106" s="2">
+      <c r="A106" s="2">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1">
         <v>275190.25</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="1">
-        <v>45397</v>
-      </c>
-      <c r="B107" s="2">
+      <c r="A107" s="2">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1">
         <v>180823</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="1">
-        <v>45398</v>
-      </c>
-      <c r="B108" s="2">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1">
         <v>170216</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="1">
-        <v>45399</v>
-      </c>
-      <c r="B109" s="2">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1">
         <v>201029</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="1">
-        <v>45400</v>
-      </c>
-      <c r="B110" s="2">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1">
         <v>229827</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="1">
-        <v>45401</v>
-      </c>
-      <c r="B111" s="2">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1">
         <v>109912.5</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="1">
-        <v>45402</v>
-      </c>
-      <c r="B112" s="2">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1">
         <v>207170.5</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="1">
-        <v>45403</v>
-      </c>
-      <c r="B113" s="2">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1">
         <v>207088.75</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="1">
-        <v>45404</v>
-      </c>
-      <c r="B114" s="2">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1">
         <v>243445.25</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="1">
-        <v>45405</v>
-      </c>
-      <c r="B115" s="2">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1">
         <v>246155.5</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="1">
-        <v>45406</v>
-      </c>
-      <c r="B116" s="2">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1">
         <v>203207.75</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="1">
-        <v>45407</v>
-      </c>
-      <c r="B117" s="2">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1">
         <v>215952</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="1">
-        <v>45408</v>
-      </c>
-      <c r="B118" s="2">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1">
         <v>244968.25</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="1">
-        <v>45409</v>
-      </c>
-      <c r="B119" s="2">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1">
         <v>329115.25</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="1">
-        <v>45410</v>
-      </c>
-      <c r="B120" s="2">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="1">
         <v>258821.75</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="1">
-        <v>45411</v>
-      </c>
-      <c r="B121" s="2">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="1">
         <v>322154.75</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="1">
-        <v>45412</v>
-      </c>
-      <c r="B122" s="2">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="1">
         <v>348198</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="1">
-        <v>45413</v>
-      </c>
-      <c r="B123" s="2">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123" s="1">
         <v>344996</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="1">
-        <v>45414</v>
-      </c>
-      <c r="B124" s="2">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124" s="1">
         <v>307097.75</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="1">
-        <v>45415</v>
-      </c>
-      <c r="B125" s="2">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="1">
         <v>169942</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="1">
-        <v>45416</v>
-      </c>
-      <c r="B126" s="2">
+      <c r="A126" s="2">
+        <v>125</v>
+      </c>
+      <c r="B126" s="1">
         <v>262161.25</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="1">
-        <v>45417</v>
-      </c>
-      <c r="B127" s="2">
+      <c r="A127" s="2">
+        <v>126</v>
+      </c>
+      <c r="B127" s="1">
         <v>224473.5</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="1">
-        <v>45418</v>
-      </c>
-      <c r="B128" s="2">
+      <c r="A128" s="2">
+        <v>127</v>
+      </c>
+      <c r="B128" s="1">
         <v>218977.25</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="1">
-        <v>45419</v>
-      </c>
-      <c r="B129" s="2">
+      <c r="A129" s="2">
+        <v>128</v>
+      </c>
+      <c r="B129" s="1">
         <v>174692.75</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="1">
-        <v>45420</v>
-      </c>
-      <c r="B130" s="2">
+      <c r="A130" s="2">
+        <v>129</v>
+      </c>
+      <c r="B130" s="1">
         <v>243263.5</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="1">
-        <v>45421</v>
-      </c>
-      <c r="B131" s="2">
+      <c r="A131" s="2">
+        <v>130</v>
+      </c>
+      <c r="B131" s="1">
         <v>359172.75</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="1">
-        <v>45422</v>
-      </c>
-      <c r="B132" s="2">
+      <c r="A132" s="2">
+        <v>131</v>
+      </c>
+      <c r="B132" s="1">
         <v>358070.25</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="1">
-        <v>45423</v>
-      </c>
-      <c r="B133" s="2">
+      <c r="A133" s="2">
+        <v>132</v>
+      </c>
+      <c r="B133" s="1">
         <v>360378.5</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="1">
-        <v>45424</v>
-      </c>
-      <c r="B134" s="2">
+      <c r="A134" s="2">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1">
         <v>370939.5</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="1">
-        <v>45425</v>
-      </c>
-      <c r="B135" s="2">
+      <c r="A135" s="2">
+        <v>134</v>
+      </c>
+      <c r="B135" s="1">
         <v>362755.5</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="1">
-        <v>45426</v>
-      </c>
-      <c r="B136" s="2">
+      <c r="A136" s="2">
+        <v>135</v>
+      </c>
+      <c r="B136" s="1">
         <v>386691.5</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="1">
-        <v>45427</v>
-      </c>
-      <c r="B137" s="2">
+      <c r="A137" s="2">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1">
         <v>316390.5</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="1">
-        <v>45428</v>
-      </c>
-      <c r="B138" s="2">
+      <c r="A138" s="2">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1">
         <v>286115.5</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="1">
-        <v>45429</v>
-      </c>
-      <c r="B139" s="2">
+      <c r="A139" s="2">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1">
         <v>206672.5</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="1">
-        <v>45430</v>
-      </c>
-      <c r="B140" s="2">
+      <c r="A140" s="2">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1">
         <v>257912.25</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="1">
-        <v>45431</v>
-      </c>
-      <c r="B141" s="2">
+      <c r="A141" s="2">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1">
         <v>263794.25</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="1">
-        <v>45432</v>
-      </c>
-      <c r="B142" s="2">
+      <c r="A142" s="2">
+        <v>141</v>
+      </c>
+      <c r="B142" s="1">
         <v>343176.5</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="1">
-        <v>45433</v>
-      </c>
-      <c r="B143" s="2">
+      <c r="A143" s="2">
+        <v>142</v>
+      </c>
+      <c r="B143" s="1">
         <v>226712.75</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="1">
-        <v>45434</v>
-      </c>
-      <c r="B144" s="2">
+      <c r="A144" s="2">
+        <v>143</v>
+      </c>
+      <c r="B144" s="1">
         <v>199077.25</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="1">
-        <v>45435</v>
-      </c>
-      <c r="B145" s="2">
+      <c r="A145" s="2">
+        <v>144</v>
+      </c>
+      <c r="B145" s="1">
         <v>303209.5</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="1">
-        <v>45436</v>
-      </c>
-      <c r="B146" s="2">
+      <c r="A146" s="2">
+        <v>145</v>
+      </c>
+      <c r="B146" s="1">
         <v>248880.5</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="1">
-        <v>45437</v>
-      </c>
-      <c r="B147" s="2">
+      <c r="A147" s="2">
+        <v>146</v>
+      </c>
+      <c r="B147" s="1">
         <v>291859.25</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="1">
-        <v>45438</v>
-      </c>
-      <c r="B148" s="2">
+      <c r="A148" s="2">
+        <v>147</v>
+      </c>
+      <c r="B148" s="1">
         <v>335599.5</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="1">
-        <v>45439</v>
-      </c>
-      <c r="B149" s="2">
+      <c r="A149" s="2">
+        <v>148</v>
+      </c>
+      <c r="B149" s="1">
         <v>269016</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="1">
-        <v>45440</v>
-      </c>
-      <c r="B150" s="2">
+      <c r="A150" s="2">
+        <v>149</v>
+      </c>
+      <c r="B150" s="1">
         <v>264086.25</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="1">
-        <v>45441</v>
-      </c>
-      <c r="B151" s="2">
+      <c r="A151" s="2">
+        <v>150</v>
+      </c>
+      <c r="B151" s="1">
         <v>227004.75</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="1">
-        <v>45442</v>
-      </c>
-      <c r="B152" s="2">
+      <c r="A152" s="2">
+        <v>151</v>
+      </c>
+      <c r="B152" s="1">
         <v>233775.75</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="1">
-        <v>45443</v>
-      </c>
-      <c r="B153" s="2">
+      <c r="A153" s="2">
+        <v>152</v>
+      </c>
+      <c r="B153" s="1">
         <v>186835.25</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="1">
-        <v>45444</v>
-      </c>
-      <c r="B154" s="2">
+      <c r="A154" s="2">
+        <v>153</v>
+      </c>
+      <c r="B154" s="1">
         <v>197548</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="1">
-        <v>45445</v>
-      </c>
-      <c r="B155" s="2">
+      <c r="A155" s="2">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1">
         <v>192727.75</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="1">
-        <v>45446</v>
-      </c>
-      <c r="B156" s="2">
+      <c r="A156" s="2">
+        <v>155</v>
+      </c>
+      <c r="B156" s="1">
         <v>189312</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="1">
-        <v>45447</v>
-      </c>
-      <c r="B157" s="2">
+      <c r="A157" s="2">
+        <v>156</v>
+      </c>
+      <c r="B157" s="1">
         <v>307375.25</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="1">
-        <v>45448</v>
-      </c>
-      <c r="B158" s="2">
+      <c r="A158" s="2">
+        <v>157</v>
+      </c>
+      <c r="B158" s="1">
         <v>259044.5</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="1">
-        <v>45449</v>
-      </c>
-      <c r="B159" s="2">
+      <c r="A159" s="2">
+        <v>158</v>
+      </c>
+      <c r="B159" s="1">
         <v>355843.5</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="1">
-        <v>45450</v>
-      </c>
-      <c r="B160" s="2">
+      <c r="A160" s="2">
+        <v>159</v>
+      </c>
+      <c r="B160" s="1">
         <v>353338</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="1">
-        <v>45451</v>
-      </c>
-      <c r="B161" s="2">
+      <c r="A161" s="2">
+        <v>160</v>
+      </c>
+      <c r="B161" s="1">
         <v>345613.5</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="1">
-        <v>45452</v>
-      </c>
-      <c r="B162" s="2">
+      <c r="A162" s="2">
+        <v>161</v>
+      </c>
+      <c r="B162" s="1">
         <v>325645.25</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="1">
-        <v>45453</v>
-      </c>
-      <c r="B163" s="2">
+      <c r="A163" s="2">
+        <v>162</v>
+      </c>
+      <c r="B163" s="1">
         <v>287234.5</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="1">
-        <v>45454</v>
-      </c>
-      <c r="B164" s="2">
+      <c r="A164" s="2">
+        <v>163</v>
+      </c>
+      <c r="B164" s="1">
         <v>263768.75</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="1">
-        <v>45455</v>
-      </c>
-      <c r="B165" s="2">
+      <c r="A165" s="2">
+        <v>164</v>
+      </c>
+      <c r="B165" s="1">
         <v>318229.75</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="1">
-        <v>45456</v>
-      </c>
-      <c r="B166" s="2">
+      <c r="A166" s="2">
+        <v>165</v>
+      </c>
+      <c r="B166" s="1">
         <v>328496.75</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="1">
-        <v>45457</v>
-      </c>
-      <c r="B167" s="2">
+      <c r="A167" s="2">
+        <v>166</v>
+      </c>
+      <c r="B167" s="1">
         <v>202570.5</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="1">
-        <v>45458</v>
-      </c>
-      <c r="B168" s="2">
+      <c r="A168" s="2">
+        <v>167</v>
+      </c>
+      <c r="B168" s="1">
         <v>262553.5</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="1">
-        <v>45459</v>
-      </c>
-      <c r="B169" s="2">
+      <c r="A169" s="2">
+        <v>168</v>
+      </c>
+      <c r="B169" s="1">
         <v>303790.75</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="1">
-        <v>45460</v>
-      </c>
-      <c r="B170" s="2">
+      <c r="A170" s="2">
+        <v>169</v>
+      </c>
+      <c r="B170" s="1">
         <v>282171.25</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="1">
-        <v>45461</v>
-      </c>
-      <c r="B171" s="2">
+      <c r="A171" s="2">
+        <v>170</v>
+      </c>
+      <c r="B171" s="1">
         <v>313482.75</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="1">
-        <v>45462</v>
-      </c>
-      <c r="B172" s="2">
+      <c r="A172" s="2">
+        <v>171</v>
+      </c>
+      <c r="B172" s="1">
         <v>248734.75</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="1">
-        <v>45463</v>
-      </c>
-      <c r="B173" s="2">
+      <c r="A173" s="2">
+        <v>172</v>
+      </c>
+      <c r="B173" s="1">
         <v>293987.5</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="1">
-        <v>45464</v>
-      </c>
-      <c r="B174" s="2">
+      <c r="A174" s="2">
+        <v>173</v>
+      </c>
+      <c r="B174" s="1">
         <v>187989</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="1">
-        <v>45465</v>
-      </c>
-      <c r="B175" s="2">
+      <c r="A175" s="2">
+        <v>174</v>
+      </c>
+      <c r="B175" s="1">
         <v>301343.75</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="1">
-        <v>45466</v>
-      </c>
-      <c r="B176" s="2">
+      <c r="A176" s="2">
+        <v>175</v>
+      </c>
+      <c r="B176" s="1">
         <v>311083.75</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" s="1">
-        <v>45467</v>
-      </c>
-      <c r="B177" s="2">
+      <c r="A177" s="2">
+        <v>176</v>
+      </c>
+      <c r="B177" s="1">
         <v>393079.25</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="1">
-        <v>45468</v>
-      </c>
-      <c r="B178" s="2">
+      <c r="A178" s="2">
+        <v>177</v>
+      </c>
+      <c r="B178" s="1">
         <v>423683.5</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" s="1">
-        <v>45469</v>
-      </c>
-      <c r="B179" s="2">
+      <c r="A179" s="2">
+        <v>178</v>
+      </c>
+      <c r="B179" s="1">
         <v>374690.5</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" s="1">
-        <v>45470</v>
-      </c>
-      <c r="B180" s="2">
+      <c r="A180" s="2">
+        <v>179</v>
+      </c>
+      <c r="B180" s="1">
         <v>319052.25</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A181" s="1">
-        <v>45471</v>
-      </c>
-      <c r="B181" s="2">
+      <c r="A181" s="2">
+        <v>180</v>
+      </c>
+      <c r="B181" s="1">
         <v>349246</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" s="1">
-        <v>45472</v>
-      </c>
-      <c r="B182" s="2">
+      <c r="A182" s="2">
+        <v>181</v>
+      </c>
+      <c r="B182" s="1">
         <v>374780.75</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" s="1">
-        <v>45473</v>
-      </c>
-      <c r="B183" s="2">
+      <c r="A183" s="2">
+        <v>182</v>
+      </c>
+      <c r="B183" s="1">
         <v>169207.25</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" s="1">
-        <v>45474</v>
-      </c>
-      <c r="B184" s="2">
+      <c r="A184" s="2">
+        <v>183</v>
+      </c>
+      <c r="B184" s="1">
         <v>224484</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" s="1">
-        <v>45475</v>
-      </c>
-      <c r="B185" s="2">
+      <c r="A185" s="2">
+        <v>184</v>
+      </c>
+      <c r="B185" s="1">
         <v>171347.75</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" s="1">
-        <v>45476</v>
-      </c>
-      <c r="B186" s="2">
+      <c r="A186" s="2">
+        <v>185</v>
+      </c>
+      <c r="B186" s="1">
         <v>197481.5</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A187" s="1">
-        <v>45477</v>
-      </c>
-      <c r="B187" s="2">
+      <c r="A187" s="2">
+        <v>186</v>
+      </c>
+      <c r="B187" s="1">
         <v>247011</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" s="1">
-        <v>45478</v>
-      </c>
-      <c r="B188" s="2">
+      <c r="A188" s="2">
+        <v>187</v>
+      </c>
+      <c r="B188" s="1">
         <v>301877.5</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A189" s="1">
-        <v>45479</v>
-      </c>
-      <c r="B189" s="2">
+      <c r="A189" s="2">
+        <v>188</v>
+      </c>
+      <c r="B189" s="1">
         <v>278181.25</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" s="1">
-        <v>45480</v>
-      </c>
-      <c r="B190" s="2">
+      <c r="A190" s="2">
+        <v>189</v>
+      </c>
+      <c r="B190" s="1">
         <v>304068.75</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A191" s="1">
-        <v>45481</v>
-      </c>
-      <c r="B191" s="2">
+      <c r="A191" s="2">
+        <v>190</v>
+      </c>
+      <c r="B191" s="1">
         <v>371343.75</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A192" s="1">
-        <v>45482</v>
-      </c>
-      <c r="B192" s="2">
+      <c r="A192" s="2">
+        <v>191</v>
+      </c>
+      <c r="B192" s="1">
         <v>401374.25</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A193" s="1">
-        <v>45483</v>
-      </c>
-      <c r="B193" s="2">
+      <c r="A193" s="2">
+        <v>192</v>
+      </c>
+      <c r="B193" s="1">
         <v>255736.75</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A194" s="1">
-        <v>45484</v>
-      </c>
-      <c r="B194" s="2">
+      <c r="A194" s="2">
+        <v>193</v>
+      </c>
+      <c r="B194" s="1">
         <v>313332.5</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A195" s="1">
-        <v>45485</v>
-      </c>
-      <c r="B195" s="2">
+      <c r="A195" s="2">
+        <v>194</v>
+      </c>
+      <c r="B195" s="1">
         <v>208798.25</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A196" s="1">
-        <v>45486</v>
-      </c>
-      <c r="B196" s="2">
+      <c r="A196" s="2">
+        <v>195</v>
+      </c>
+      <c r="B196" s="1">
         <v>263030.25</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A197" s="1">
-        <v>45487</v>
-      </c>
-      <c r="B197" s="2">
+      <c r="A197" s="2">
+        <v>196</v>
+      </c>
+      <c r="B197" s="1">
         <v>335793</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A198" s="1">
-        <v>45488</v>
-      </c>
-      <c r="B198" s="2">
+      <c r="A198" s="2">
+        <v>197</v>
+      </c>
+      <c r="B198" s="1">
         <v>389618.25</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A199" s="1">
-        <v>45489</v>
-      </c>
-      <c r="B199" s="2">
+      <c r="A199" s="2">
+        <v>198</v>
+      </c>
+      <c r="B199" s="1">
         <v>274708</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="1">
-        <v>45490</v>
-      </c>
-      <c r="B200" s="2">
+      <c r="A200" s="2">
+        <v>199</v>
+      </c>
+      <c r="B200" s="1">
         <v>267626.25</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" s="1">
-        <v>45491</v>
-      </c>
-      <c r="B201" s="2">
+      <c r="A201" s="2">
+        <v>200</v>
+      </c>
+      <c r="B201" s="1">
         <v>374080.25</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="1">
-        <v>45492</v>
-      </c>
-      <c r="B202" s="2">
+      <c r="A202" s="2">
+        <v>201</v>
+      </c>
+      <c r="B202" s="1">
         <v>367167.25</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="1">
-        <v>45493</v>
-      </c>
-      <c r="B203" s="2">
+      <c r="A203" s="2">
+        <v>202</v>
+      </c>
+      <c r="B203" s="1">
         <v>366124.25</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="1">
-        <v>45494</v>
-      </c>
-      <c r="B204" s="2">
+      <c r="A204" s="2">
+        <v>203</v>
+      </c>
+      <c r="B204" s="1">
         <v>308987.75</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A205" s="1">
-        <v>45495</v>
-      </c>
-      <c r="B205" s="2">
+      <c r="A205" s="2">
+        <v>204</v>
+      </c>
+      <c r="B205" s="1">
         <v>276683.25</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="1">
-        <v>45496</v>
-      </c>
-      <c r="B206" s="2">
+      <c r="A206" s="2">
+        <v>205</v>
+      </c>
+      <c r="B206" s="1">
         <v>266456.5</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="1">
-        <v>45497</v>
-      </c>
-      <c r="B207" s="2">
+      <c r="A207" s="2">
+        <v>206</v>
+      </c>
+      <c r="B207" s="1">
         <v>293321</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="1">
-        <v>45498</v>
-      </c>
-      <c r="B208" s="2">
+      <c r="A208" s="2">
+        <v>207</v>
+      </c>
+      <c r="B208" s="1">
         <v>357772.25</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="1">
-        <v>45499</v>
-      </c>
-      <c r="B209" s="2">
+      <c r="A209" s="2">
+        <v>208</v>
+      </c>
+      <c r="B209" s="1">
         <v>228982.5</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="1">
-        <v>45500</v>
-      </c>
-      <c r="B210" s="2">
+      <c r="A210" s="2">
+        <v>209</v>
+      </c>
+      <c r="B210" s="1">
         <v>220503</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="1">
-        <v>45501</v>
-      </c>
-      <c r="B211" s="2">
+      <c r="A211" s="2">
+        <v>210</v>
+      </c>
+      <c r="B211" s="1">
         <v>313645</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="1">
-        <v>45502</v>
-      </c>
-      <c r="B212" s="2">
+      <c r="A212" s="2">
+        <v>211</v>
+      </c>
+      <c r="B212" s="1">
         <v>405747.75</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="1">
-        <v>45503</v>
-      </c>
-      <c r="B213" s="2">
+      <c r="A213" s="2">
+        <v>212</v>
+      </c>
+      <c r="B213" s="1">
         <v>394049</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="1">
-        <v>45504</v>
-      </c>
-      <c r="B214" s="2">
+      <c r="A214" s="2">
+        <v>213</v>
+      </c>
+      <c r="B214" s="1">
         <v>327485</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="1">
-        <v>45505</v>
-      </c>
-      <c r="B215" s="2">
+      <c r="A215" s="2">
+        <v>214</v>
+      </c>
+      <c r="B215" s="1">
         <v>265180.75</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="1">
-        <v>45506</v>
-      </c>
-      <c r="B216" s="2">
+      <c r="A216" s="2">
+        <v>215</v>
+      </c>
+      <c r="B216" s="1">
         <v>242089.75</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="1">
-        <v>45507</v>
-      </c>
-      <c r="B217" s="2">
+      <c r="A217" s="2">
+        <v>216</v>
+      </c>
+      <c r="B217" s="1">
         <v>301755.5</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="1">
-        <v>45508</v>
-      </c>
-      <c r="B218" s="2">
+      <c r="A218" s="2">
+        <v>217</v>
+      </c>
+      <c r="B218" s="1">
         <v>241460</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="1">
-        <v>45509</v>
-      </c>
-      <c r="B219" s="2">
+      <c r="A219" s="2">
+        <v>218</v>
+      </c>
+      <c r="B219" s="1">
         <v>313359.25</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="1">
-        <v>45510</v>
-      </c>
-      <c r="B220" s="2">
+      <c r="A220" s="2">
+        <v>219</v>
+      </c>
+      <c r="B220" s="1">
         <v>381126.75</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="1">
-        <v>45511</v>
-      </c>
-      <c r="B221" s="2">
+      <c r="A221" s="2">
+        <v>220</v>
+      </c>
+      <c r="B221" s="1">
         <v>269186.5</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="1">
-        <v>45512</v>
-      </c>
-      <c r="B222" s="2">
+      <c r="A222" s="2">
+        <v>221</v>
+      </c>
+      <c r="B222" s="1">
         <v>255391.25</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="1">
-        <v>45513</v>
-      </c>
-      <c r="B223" s="2">
+      <c r="A223" s="2">
+        <v>222</v>
+      </c>
+      <c r="B223" s="1">
         <v>249689.75</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="1">
-        <v>45514</v>
-      </c>
-      <c r="B224" s="2">
+      <c r="A224" s="2">
+        <v>223</v>
+      </c>
+      <c r="B224" s="1">
         <v>335573.25</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="1">
-        <v>45515</v>
-      </c>
-      <c r="B225" s="2">
+      <c r="A225" s="2">
+        <v>224</v>
+      </c>
+      <c r="B225" s="1">
         <v>353144</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="1">
-        <v>45516</v>
-      </c>
-      <c r="B226" s="2">
+      <c r="A226" s="2">
+        <v>225</v>
+      </c>
+      <c r="B226" s="1">
         <v>363243.5</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" s="1">
-        <v>45517</v>
-      </c>
-      <c r="B227" s="2">
+      <c r="A227" s="2">
+        <v>226</v>
+      </c>
+      <c r="B227" s="1">
         <v>340536.25</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="1">
-        <v>45518</v>
-      </c>
-      <c r="B228" s="2">
+      <c r="A228" s="2">
+        <v>227</v>
+      </c>
+      <c r="B228" s="1">
         <v>281910</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A229" s="1">
-        <v>45519</v>
-      </c>
-      <c r="B229" s="2">
+      <c r="A229" s="2">
+        <v>228</v>
+      </c>
+      <c r="B229" s="1">
         <v>307704.75</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="1">
-        <v>45520</v>
-      </c>
-      <c r="B230" s="2">
+      <c r="A230" s="2">
+        <v>229</v>
+      </c>
+      <c r="B230" s="1">
         <v>291358.5</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A231" s="1">
-        <v>45521</v>
-      </c>
-      <c r="B231" s="2">
+      <c r="A231" s="2">
+        <v>230</v>
+      </c>
+      <c r="B231" s="1">
         <v>242398.25</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="1">
-        <v>45522</v>
-      </c>
-      <c r="B232" s="2">
+      <c r="A232" s="2">
+        <v>231</v>
+      </c>
+      <c r="B232" s="1">
         <v>143567.75</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A233" s="1">
-        <v>45523</v>
-      </c>
-      <c r="B233" s="2">
+      <c r="A233" s="2">
+        <v>232</v>
+      </c>
+      <c r="B233" s="1">
         <v>242218.75</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A234" s="1">
-        <v>45524</v>
-      </c>
-      <c r="B234" s="2">
+      <c r="A234" s="2">
+        <v>233</v>
+      </c>
+      <c r="B234" s="1">
         <v>263964.5</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A235" s="1">
-        <v>45525</v>
-      </c>
-      <c r="B235" s="2">
+      <c r="A235" s="2">
+        <v>234</v>
+      </c>
+      <c r="B235" s="1">
         <v>272153.5</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" s="1">
-        <v>45526</v>
-      </c>
-      <c r="B236" s="2">
+      <c r="A236" s="2">
+        <v>235</v>
+      </c>
+      <c r="B236" s="1">
         <v>304486</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A237" s="1">
-        <v>45527</v>
-      </c>
-      <c r="B237" s="2">
+      <c r="A237" s="2">
+        <v>236</v>
+      </c>
+      <c r="B237" s="1">
         <v>292807.5</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A238" s="1">
-        <v>45528</v>
-      </c>
-      <c r="B238" s="2">
+      <c r="A238" s="2">
+        <v>237</v>
+      </c>
+      <c r="B238" s="1">
         <v>329105.75</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A239" s="1">
-        <v>45529</v>
-      </c>
-      <c r="B239" s="2">
+      <c r="A239" s="2">
+        <v>238</v>
+      </c>
+      <c r="B239" s="1">
         <v>220099</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A240" s="1">
-        <v>45530</v>
-      </c>
-      <c r="B240" s="2">
+      <c r="A240" s="2">
+        <v>239</v>
+      </c>
+      <c r="B240" s="1">
         <v>277325.5</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A241" s="1">
-        <v>45531</v>
-      </c>
-      <c r="B241" s="2">
+      <c r="A241" s="2">
+        <v>240</v>
+      </c>
+      <c r="B241" s="1">
         <v>337559.75</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" s="1">
-        <v>45532</v>
-      </c>
-      <c r="B242" s="2">
+      <c r="A242" s="2">
+        <v>241</v>
+      </c>
+      <c r="B242" s="1">
         <v>343097</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" s="1">
-        <v>45533</v>
-      </c>
-      <c r="B243" s="2">
+      <c r="A243" s="2">
+        <v>242</v>
+      </c>
+      <c r="B243" s="1">
         <v>322183</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" s="1">
-        <v>45534</v>
-      </c>
-      <c r="B244" s="2">
+      <c r="A244" s="2">
+        <v>243</v>
+      </c>
+      <c r="B244" s="1">
         <v>253418</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" s="1">
-        <v>45535</v>
-      </c>
-      <c r="B245" s="2">
+      <c r="A245" s="2">
+        <v>244</v>
+      </c>
+      <c r="B245" s="1">
         <v>303968.25</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" s="1">
-        <v>45536</v>
-      </c>
-      <c r="B246" s="2">
+      <c r="A246" s="2">
+        <v>245</v>
+      </c>
+      <c r="B246" s="1">
         <v>316098</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A247" s="1">
-        <v>45537</v>
-      </c>
-      <c r="B247" s="2">
+      <c r="A247" s="2">
+        <v>246</v>
+      </c>
+      <c r="B247" s="1">
         <v>264715.5</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A248" s="1">
-        <v>45538</v>
-      </c>
-      <c r="B248" s="2">
+      <c r="A248" s="2">
+        <v>247</v>
+      </c>
+      <c r="B248" s="1">
         <v>276921</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A249" s="1">
-        <v>45539</v>
-      </c>
-      <c r="B249" s="2">
+      <c r="A249" s="2">
+        <v>248</v>
+      </c>
+      <c r="B249" s="1">
         <v>223443.75</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A250" s="1">
-        <v>45540</v>
-      </c>
-      <c r="B250" s="2">
+      <c r="A250" s="2">
+        <v>249</v>
+      </c>
+      <c r="B250" s="1">
         <v>284865.25</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A251" s="1">
-        <v>45541</v>
-      </c>
-      <c r="B251" s="2">
+      <c r="A251" s="2">
+        <v>250</v>
+      </c>
+      <c r="B251" s="1">
         <v>239113.75</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A252" s="1">
-        <v>45542</v>
-      </c>
-      <c r="B252" s="2">
+      <c r="A252" s="2">
+        <v>251</v>
+      </c>
+      <c r="B252" s="1">
         <v>307149</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A253" s="1">
-        <v>45543</v>
-      </c>
-      <c r="B253" s="2">
+      <c r="A253" s="2">
+        <v>252</v>
+      </c>
+      <c r="B253" s="1">
         <v>210696.25</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A254" s="1">
-        <v>45544</v>
-      </c>
-      <c r="B254" s="2">
+      <c r="A254" s="2">
+        <v>253</v>
+      </c>
+      <c r="B254" s="1">
         <v>129942.25</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A255" s="1">
-        <v>45545</v>
-      </c>
-      <c r="B255" s="2">
+      <c r="A255" s="2">
+        <v>254</v>
+      </c>
+      <c r="B255" s="1">
         <v>175796.75</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A256" s="1">
-        <v>45546</v>
-      </c>
-      <c r="B256" s="2">
+      <c r="A256" s="2">
+        <v>255</v>
+      </c>
+      <c r="B256" s="1">
         <v>134425.75</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A257" s="1">
-        <v>45547</v>
-      </c>
-      <c r="B257" s="2">
+      <c r="A257" s="2">
+        <v>256</v>
+      </c>
+      <c r="B257" s="1">
         <v>199073</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A258" s="1">
-        <v>45548</v>
-      </c>
-      <c r="B258" s="2">
+      <c r="A258" s="2">
+        <v>257</v>
+      </c>
+      <c r="B258" s="1">
         <v>149067</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A259" s="1">
-        <v>45549</v>
-      </c>
-      <c r="B259" s="2">
+      <c r="A259" s="2">
+        <v>258</v>
+      </c>
+      <c r="B259" s="1">
         <v>178593.75</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A260" s="1">
-        <v>45550</v>
-      </c>
-      <c r="B260" s="2">
+      <c r="A260" s="2">
+        <v>259</v>
+      </c>
+      <c r="B260" s="1">
         <v>221483.25</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A261" s="1">
-        <v>45551</v>
-      </c>
-      <c r="B261" s="2">
+      <c r="A261" s="2">
+        <v>260</v>
+      </c>
+      <c r="B261" s="1">
         <v>85603.5</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A262" s="1">
-        <v>45552</v>
-      </c>
-      <c r="B262" s="2">
+      <c r="A262" s="2">
+        <v>261</v>
+      </c>
+      <c r="B262" s="1">
         <v>185705</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A263" s="1">
-        <v>45553</v>
-      </c>
-      <c r="B263" s="2">
+      <c r="A263" s="2">
+        <v>262</v>
+      </c>
+      <c r="B263" s="1">
         <v>250812.5</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A264" s="1">
-        <v>45554</v>
-      </c>
-      <c r="B264" s="2">
+      <c r="A264" s="2">
+        <v>263</v>
+      </c>
+      <c r="B264" s="1">
         <v>249788.25</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A265" s="1">
-        <v>45555</v>
-      </c>
-      <c r="B265" s="2">
+      <c r="A265" s="2">
+        <v>264</v>
+      </c>
+      <c r="B265" s="1">
         <v>288421.25</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A266" s="1">
-        <v>45556</v>
-      </c>
-      <c r="B266" s="2">
+      <c r="A266" s="2">
+        <v>265</v>
+      </c>
+      <c r="B266" s="1">
         <v>293237.25</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A267" s="1">
-        <v>45557</v>
-      </c>
-      <c r="B267" s="2">
+      <c r="A267" s="2">
+        <v>266</v>
+      </c>
+      <c r="B267" s="1">
         <v>255268.25</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A268" s="1">
-        <v>45558</v>
-      </c>
-      <c r="B268" s="2">
+      <c r="A268" s="2">
+        <v>267</v>
+      </c>
+      <c r="B268" s="1">
         <v>184974</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A269" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B269" s="2">
+      <c r="A269" s="2">
+        <v>268</v>
+      </c>
+      <c r="B269" s="1">
         <v>139403.25</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A270" s="1">
-        <v>45560</v>
-      </c>
-      <c r="B270" s="2">
+      <c r="A270" s="2">
+        <v>269</v>
+      </c>
+      <c r="B270" s="1">
         <v>140983.75</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A271" s="1">
-        <v>45561</v>
-      </c>
-      <c r="B271" s="2">
+      <c r="A271" s="2">
+        <v>270</v>
+      </c>
+      <c r="B271" s="1">
         <v>64990.5</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A272" s="1">
-        <v>45562</v>
-      </c>
-      <c r="B272" s="2">
+      <c r="A272" s="2">
+        <v>271</v>
+      </c>
+      <c r="B272" s="1">
         <v>153642.75</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A273" s="1">
-        <v>45563</v>
-      </c>
-      <c r="B273" s="2">
+      <c r="A273" s="2">
+        <v>272</v>
+      </c>
+      <c r="B273" s="1">
         <v>175221.75</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A274" s="1">
-        <v>45564</v>
-      </c>
-      <c r="B274" s="2">
+      <c r="A274" s="2">
+        <v>273</v>
+      </c>
+      <c r="B274" s="1">
         <v>229217.25</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A275" s="1">
-        <v>45565</v>
-      </c>
-      <c r="B275" s="2">
+      <c r="A275" s="2">
+        <v>274</v>
+      </c>
+      <c r="B275" s="1">
         <v>152664</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A276" s="1">
-        <v>45566</v>
-      </c>
-      <c r="B276" s="2">
+      <c r="A276" s="2">
+        <v>275</v>
+      </c>
+      <c r="B276" s="1">
         <v>106277.5</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A277" s="1">
-        <v>45567</v>
-      </c>
-      <c r="B277" s="2">
+      <c r="A277" s="2">
+        <v>276</v>
+      </c>
+      <c r="B277" s="1">
         <v>95404.75</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A278" s="1">
-        <v>45568</v>
-      </c>
-      <c r="B278" s="2">
+      <c r="A278" s="2">
+        <v>277</v>
+      </c>
+      <c r="B278" s="1">
         <v>99557.75</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A279" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B279" s="2">
+      <c r="A279" s="2">
+        <v>278</v>
+      </c>
+      <c r="B279" s="1">
         <v>117274</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A280" s="1">
-        <v>45570</v>
-      </c>
-      <c r="B280" s="2">
+      <c r="A280" s="2">
+        <v>279</v>
+      </c>
+      <c r="B280" s="1">
         <v>138643</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A281" s="1">
-        <v>45571</v>
-      </c>
-      <c r="B281" s="2">
+      <c r="A281" s="2">
+        <v>280</v>
+      </c>
+      <c r="B281" s="1">
         <v>167337.25</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A282" s="1">
-        <v>45572</v>
-      </c>
-      <c r="B282" s="2">
+      <c r="A282" s="2">
+        <v>281</v>
+      </c>
+      <c r="B282" s="1">
         <v>126711.75</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A283" s="1">
-        <v>45573</v>
-      </c>
-      <c r="B283" s="2">
+      <c r="A283" s="2">
+        <v>282</v>
+      </c>
+      <c r="B283" s="1">
         <v>106363.25</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A284" s="1">
-        <v>45574</v>
-      </c>
-      <c r="B284" s="2">
+      <c r="A284" s="2">
+        <v>283</v>
+      </c>
+      <c r="B284" s="1">
         <v>136812.5</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A285" s="1">
-        <v>45575</v>
-      </c>
-      <c r="B285" s="2">
+      <c r="A285" s="2">
+        <v>284</v>
+      </c>
+      <c r="B285" s="1">
         <v>84860.25</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A286" s="1">
-        <v>45576</v>
-      </c>
-      <c r="B286" s="2">
+      <c r="A286" s="2">
+        <v>285</v>
+      </c>
+      <c r="B286" s="1">
         <v>158195.25</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A287" s="1">
-        <v>45577</v>
-      </c>
-      <c r="B287" s="2">
+      <c r="A287" s="2">
+        <v>286</v>
+      </c>
+      <c r="B287" s="1">
         <v>157191.25</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A288" s="1">
-        <v>45578</v>
-      </c>
-      <c r="B288" s="2">
+      <c r="A288" s="2">
+        <v>287</v>
+      </c>
+      <c r="B288" s="1">
         <v>121182.25</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A289" s="1">
-        <v>45579</v>
-      </c>
-      <c r="B289" s="2">
+      <c r="A289" s="2">
+        <v>288</v>
+      </c>
+      <c r="B289" s="1">
         <v>97194.25</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A290" s="1">
-        <v>45580</v>
-      </c>
-      <c r="B290" s="2">
+      <c r="A290" s="2">
+        <v>289</v>
+      </c>
+      <c r="B290" s="1">
         <v>140780.75</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A291" s="1">
-        <v>45581</v>
-      </c>
-      <c r="B291" s="2">
+      <c r="A291" s="2">
+        <v>290</v>
+      </c>
+      <c r="B291" s="1">
         <v>166541.75</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A292" s="1">
-        <v>45582</v>
-      </c>
-      <c r="B292" s="2">
+      <c r="A292" s="2">
+        <v>291</v>
+      </c>
+      <c r="B292" s="1">
         <v>150831.25</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A293" s="1">
-        <v>45583</v>
-      </c>
-      <c r="B293" s="2">
+      <c r="A293" s="2">
+        <v>292</v>
+      </c>
+      <c r="B293" s="1">
         <v>113393.25</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A294" s="1">
-        <v>45584</v>
-      </c>
-      <c r="B294" s="2">
+      <c r="A294" s="2">
+        <v>293</v>
+      </c>
+      <c r="B294" s="1">
         <v>89614</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A295" s="1">
-        <v>45585</v>
-      </c>
-      <c r="B295" s="2">
+      <c r="A295" s="2">
+        <v>294</v>
+      </c>
+      <c r="B295" s="1">
         <v>112994</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A296" s="1">
-        <v>45586</v>
-      </c>
-      <c r="B296" s="2">
+      <c r="A296" s="2">
+        <v>295</v>
+      </c>
+      <c r="B296" s="1">
         <v>107509</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A297" s="1">
-        <v>45587</v>
-      </c>
-      <c r="B297" s="2">
+      <c r="A297" s="2">
+        <v>296</v>
+      </c>
+      <c r="B297" s="1">
         <v>101380.5</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A298" s="1">
-        <v>45588</v>
-      </c>
-      <c r="B298" s="2">
+      <c r="A298" s="2">
+        <v>297</v>
+      </c>
+      <c r="B298" s="1">
         <v>122734.75</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A299" s="1">
-        <v>45589</v>
-      </c>
-      <c r="B299" s="2">
+      <c r="A299" s="2">
+        <v>298</v>
+      </c>
+      <c r="B299" s="1">
         <v>110466.25</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A300" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B300" s="2">
+      <c r="A300" s="2">
+        <v>299</v>
+      </c>
+      <c r="B300" s="1">
         <v>138203.25</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A301" s="1">
-        <v>45591</v>
-      </c>
-      <c r="B301" s="2">
+      <c r="A301" s="2">
+        <v>300</v>
+      </c>
+      <c r="B301" s="1">
         <v>125770.5</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A302" s="1">
-        <v>45592</v>
-      </c>
-      <c r="B302" s="2">
+      <c r="A302" s="2">
+        <v>301</v>
+      </c>
+      <c r="B302" s="1">
         <v>84347.25</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A303" s="1">
-        <v>45593</v>
-      </c>
-      <c r="B303" s="2">
+      <c r="A303" s="2">
+        <v>302</v>
+      </c>
+      <c r="B303" s="1">
         <v>88838.5</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A304" s="1">
-        <v>45594</v>
-      </c>
-      <c r="B304" s="2">
+      <c r="A304" s="2">
+        <v>303</v>
+      </c>
+      <c r="B304" s="1">
         <v>85994.5</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A305" s="1">
-        <v>45595</v>
-      </c>
-      <c r="B305" s="2">
+      <c r="A305" s="2">
+        <v>304</v>
+      </c>
+      <c r="B305" s="1">
         <v>63374.5</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A306" s="1">
-        <v>45596</v>
-      </c>
-      <c r="B306" s="2">
+      <c r="A306" s="2">
+        <v>305</v>
+      </c>
+      <c r="B306" s="1">
         <v>45791.5</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A307" s="1">
-        <v>45597</v>
-      </c>
-      <c r="B307" s="2">
+      <c r="A307" s="2">
+        <v>306</v>
+      </c>
+      <c r="B307" s="1">
         <v>63610</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A308" s="1">
-        <v>45598</v>
-      </c>
-      <c r="B308" s="2">
+      <c r="A308" s="2">
+        <v>307</v>
+      </c>
+      <c r="B308" s="1">
         <v>71585</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A309" s="1">
-        <v>45599</v>
-      </c>
-      <c r="B309" s="2">
+      <c r="A309" s="2">
+        <v>308</v>
+      </c>
+      <c r="B309" s="1">
         <v>129997</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A310" s="1">
-        <v>45600</v>
-      </c>
-      <c r="B310" s="2">
+      <c r="A310" s="2">
+        <v>309</v>
+      </c>
+      <c r="B310" s="1">
         <v>86186.75</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A311" s="1">
-        <v>45601</v>
-      </c>
-      <c r="B311" s="2">
+      <c r="A311" s="2">
+        <v>310</v>
+      </c>
+      <c r="B311" s="1">
         <v>75285.5</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A312" s="1">
-        <v>45602</v>
-      </c>
-      <c r="B312" s="2">
+      <c r="A312" s="2">
+        <v>311</v>
+      </c>
+      <c r="B312" s="1">
         <v>36511.75</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A313" s="1">
-        <v>45603</v>
-      </c>
-      <c r="B313" s="2">
+      <c r="A313" s="2">
+        <v>312</v>
+      </c>
+      <c r="B313" s="1">
         <v>22467.25</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A314" s="1">
-        <v>45604</v>
-      </c>
-      <c r="B314" s="2">
+      <c r="A314" s="2">
+        <v>313</v>
+      </c>
+      <c r="B314" s="1">
         <v>22069.75</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A315" s="1">
-        <v>45605</v>
-      </c>
-      <c r="B315" s="2">
+      <c r="A315" s="2">
+        <v>314</v>
+      </c>
+      <c r="B315" s="1">
         <v>48775.25</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A316" s="1">
-        <v>45606</v>
-      </c>
-      <c r="B316" s="2">
+      <c r="A316" s="2">
+        <v>315</v>
+      </c>
+      <c r="B316" s="1">
         <v>33330.25</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A317" s="1">
-        <v>45607</v>
-      </c>
-      <c r="B317" s="2">
+      <c r="A317" s="2">
+        <v>316</v>
+      </c>
+      <c r="B317" s="1">
         <v>27821.25</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A318" s="1">
-        <v>45608</v>
-      </c>
-      <c r="B318" s="2">
+      <c r="A318" s="2">
+        <v>317</v>
+      </c>
+      <c r="B318" s="1">
         <v>30726.25</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A319" s="1">
-        <v>45609</v>
-      </c>
-      <c r="B319" s="2">
+      <c r="A319" s="2">
+        <v>318</v>
+      </c>
+      <c r="B319" s="1">
         <v>21623.75</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A320" s="1">
-        <v>45610</v>
-      </c>
-      <c r="B320" s="2">
+      <c r="A320" s="2">
+        <v>319</v>
+      </c>
+      <c r="B320" s="1">
         <v>31630.75</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A321" s="1">
-        <v>45611</v>
-      </c>
-      <c r="B321" s="2">
+      <c r="A321" s="2">
+        <v>320</v>
+      </c>
+      <c r="B321" s="1">
         <v>35148.25</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A322" s="1">
-        <v>45612</v>
-      </c>
-      <c r="B322" s="2">
+      <c r="A322" s="2">
+        <v>321</v>
+      </c>
+      <c r="B322" s="1">
         <v>48810.25</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A323" s="1">
-        <v>45613</v>
-      </c>
-      <c r="B323" s="2">
+      <c r="A323" s="2">
+        <v>322</v>
+      </c>
+      <c r="B323" s="1">
         <v>41442.25</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A324" s="1">
-        <v>45614</v>
-      </c>
-      <c r="B324" s="2">
+      <c r="A324" s="2">
+        <v>323</v>
+      </c>
+      <c r="B324" s="1">
         <v>53363.5</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A325" s="1">
-        <v>45615</v>
-      </c>
-      <c r="B325" s="2">
+      <c r="A325" s="2">
+        <v>324</v>
+      </c>
+      <c r="B325" s="1">
         <v>22367.5</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A326" s="1">
-        <v>45616</v>
-      </c>
-      <c r="B326" s="2">
+      <c r="A326" s="2">
+        <v>325</v>
+      </c>
+      <c r="B326" s="1">
         <v>48512.25</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A327" s="1">
-        <v>45617</v>
-      </c>
-      <c r="B327" s="2">
+      <c r="A327" s="2">
+        <v>326</v>
+      </c>
+      <c r="B327" s="1">
         <v>43893.5</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A328" s="1">
-        <v>45618</v>
-      </c>
-      <c r="B328" s="2">
+      <c r="A328" s="2">
+        <v>327</v>
+      </c>
+      <c r="B328" s="1">
         <v>38530.75</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A329" s="1">
-        <v>45619</v>
-      </c>
-      <c r="B329" s="2">
+      <c r="A329" s="2">
+        <v>328</v>
+      </c>
+      <c r="B329" s="1">
         <v>56596</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A330" s="1">
-        <v>45620</v>
-      </c>
-      <c r="B330" s="2">
+      <c r="A330" s="2">
+        <v>329</v>
+      </c>
+      <c r="B330" s="1">
         <v>53030.5</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A331" s="1">
-        <v>45621</v>
-      </c>
-      <c r="B331" s="2">
+      <c r="A331" s="2">
+        <v>330</v>
+      </c>
+      <c r="B331" s="1">
         <v>62641</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A332" s="1">
-        <v>45622</v>
-      </c>
-      <c r="B332" s="2">
+      <c r="A332" s="2">
+        <v>331</v>
+      </c>
+      <c r="B332" s="1">
         <v>56822.25</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A333" s="1">
-        <v>45623</v>
-      </c>
-      <c r="B333" s="2">
+      <c r="A333" s="2">
+        <v>332</v>
+      </c>
+      <c r="B333" s="1">
         <v>61229.75</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A334" s="1">
-        <v>45624</v>
-      </c>
-      <c r="B334" s="2">
+      <c r="A334" s="2">
+        <v>333</v>
+      </c>
+      <c r="B334" s="1">
         <v>34457.25</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A335" s="1">
-        <v>45625</v>
-      </c>
-      <c r="B335" s="2">
+      <c r="A335" s="2">
+        <v>334</v>
+      </c>
+      <c r="B335" s="1">
         <v>62157.25</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A336" s="1">
-        <v>45626</v>
-      </c>
-      <c r="B336" s="2">
+      <c r="A336" s="2">
+        <v>335</v>
+      </c>
+      <c r="B336" s="1">
         <v>109063.5</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A337" s="1">
-        <v>45627</v>
-      </c>
-      <c r="B337" s="2">
+      <c r="A337" s="2">
+        <v>336</v>
+      </c>
+      <c r="B337" s="1">
         <v>74638.25</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A338" s="1">
-        <v>45628</v>
-      </c>
-      <c r="B338" s="2">
+      <c r="A338" s="2">
+        <v>337</v>
+      </c>
+      <c r="B338" s="1">
         <v>29315</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A339" s="1">
-        <v>45629</v>
-      </c>
-      <c r="B339" s="2">
+      <c r="A339" s="2">
+        <v>338</v>
+      </c>
+      <c r="B339" s="1">
         <v>36936.75</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A340" s="1">
-        <v>45630</v>
-      </c>
-      <c r="B340" s="2">
+      <c r="A340" s="2">
+        <v>339</v>
+      </c>
+      <c r="B340" s="1">
         <v>36173.75</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A341" s="1">
-        <v>45631</v>
-      </c>
-      <c r="B341" s="2">
+      <c r="A341" s="2">
+        <v>340</v>
+      </c>
+      <c r="B341" s="1">
         <v>60282.25</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A342" s="1">
-        <v>45632</v>
-      </c>
-      <c r="B342" s="2">
+      <c r="A342" s="2">
+        <v>341</v>
+      </c>
+      <c r="B342" s="1">
         <v>25480</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A343" s="1">
-        <v>45633</v>
-      </c>
-      <c r="B343" s="2">
+      <c r="A343" s="2">
+        <v>342</v>
+      </c>
+      <c r="B343" s="1">
         <v>18726.25</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A344" s="1">
-        <v>45634</v>
-      </c>
-      <c r="B344" s="2">
+      <c r="A344" s="2">
+        <v>343</v>
+      </c>
+      <c r="B344" s="1">
         <v>33497.25</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A345" s="1">
-        <v>45635</v>
-      </c>
-      <c r="B345" s="2">
+      <c r="A345" s="2">
+        <v>344</v>
+      </c>
+      <c r="B345" s="1">
         <v>12305.5</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A346" s="1">
-        <v>45636</v>
-      </c>
-      <c r="B346" s="2">
+      <c r="A346" s="2">
+        <v>345</v>
+      </c>
+      <c r="B346" s="1">
         <v>12939.75</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A347" s="1">
-        <v>45637</v>
-      </c>
-      <c r="B347" s="2">
+      <c r="A347" s="2">
+        <v>346</v>
+      </c>
+      <c r="B347" s="1">
         <v>12986.25</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A348" s="1">
-        <v>45638</v>
-      </c>
-      <c r="B348" s="2">
+      <c r="A348" s="2">
+        <v>347</v>
+      </c>
+      <c r="B348" s="1">
         <v>15430.75</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A349" s="1">
-        <v>45639</v>
-      </c>
-      <c r="B349" s="2">
+      <c r="A349" s="2">
+        <v>348</v>
+      </c>
+      <c r="B349" s="1">
         <v>26561.75</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A350" s="1">
-        <v>45640</v>
-      </c>
-      <c r="B350" s="2">
+      <c r="A350" s="2">
+        <v>349</v>
+      </c>
+      <c r="B350" s="1">
         <v>20081.25</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A351" s="1">
-        <v>45641</v>
-      </c>
-      <c r="B351" s="2">
+      <c r="A351" s="2">
+        <v>350</v>
+      </c>
+      <c r="B351" s="1">
         <v>24157.25</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A352" s="1">
-        <v>45642</v>
-      </c>
-      <c r="B352" s="2">
+      <c r="A352" s="2">
+        <v>351</v>
+      </c>
+      <c r="B352" s="1">
         <v>25287.75</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A353" s="1">
-        <v>45643</v>
-      </c>
-      <c r="B353" s="2">
+      <c r="A353" s="2">
+        <v>352</v>
+      </c>
+      <c r="B353" s="1">
         <v>27160</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A354" s="1">
-        <v>45644</v>
-      </c>
-      <c r="B354" s="2">
+      <c r="A354" s="2">
+        <v>353</v>
+      </c>
+      <c r="B354" s="1">
         <v>32798.5</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A355" s="1">
-        <v>45645</v>
-      </c>
-      <c r="B355" s="2">
+      <c r="A355" s="2">
+        <v>354</v>
+      </c>
+      <c r="B355" s="1">
         <v>19794.75</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A356" s="1">
-        <v>45646</v>
-      </c>
-      <c r="B356" s="2">
+      <c r="A356" s="2">
+        <v>355</v>
+      </c>
+      <c r="B356" s="1">
         <v>39862.5</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A357" s="1">
-        <v>45647</v>
-      </c>
-      <c r="B357" s="2">
+      <c r="A357" s="2">
+        <v>356</v>
+      </c>
+      <c r="B357" s="1">
         <v>30222.75</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A358" s="1">
-        <v>45648</v>
-      </c>
-      <c r="B358" s="2">
+      <c r="A358" s="2">
+        <v>357</v>
+      </c>
+      <c r="B358" s="1">
         <v>21552.75</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A359" s="1">
-        <v>45649</v>
-      </c>
-      <c r="B359" s="2">
+      <c r="A359" s="2">
+        <v>358</v>
+      </c>
+      <c r="B359" s="1">
         <v>31522.25</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A360" s="1">
-        <v>45650</v>
-      </c>
-      <c r="B360" s="2">
+      <c r="A360" s="2">
+        <v>359</v>
+      </c>
+      <c r="B360" s="1">
         <v>33799.25</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A361" s="1">
-        <v>45651</v>
-      </c>
-      <c r="B361" s="2">
+      <c r="A361" s="2">
+        <v>360</v>
+      </c>
+      <c r="B361" s="1">
         <v>48980.5</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A362" s="1">
-        <v>45652</v>
-      </c>
-      <c r="B362" s="2">
+      <c r="A362" s="2">
+        <v>361</v>
+      </c>
+      <c r="B362" s="1">
         <v>52246.75</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A363" s="1">
-        <v>45653</v>
-      </c>
-      <c r="B363" s="2">
+      <c r="A363" s="2">
+        <v>362</v>
+      </c>
+      <c r="B363" s="1">
         <v>61205.75</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A364" s="1">
-        <v>45654</v>
-      </c>
-      <c r="B364" s="2">
+      <c r="A364" s="2">
+        <v>363</v>
+      </c>
+      <c r="B364" s="1">
         <v>61088.5</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A365" s="1">
-        <v>45655</v>
-      </c>
-      <c r="B365" s="2">
+      <c r="A365" s="2">
+        <v>364</v>
+      </c>
+      <c r="B365" s="1">
         <v>39719</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A366" s="1">
-        <v>45656</v>
-      </c>
-      <c r="B366" s="2">
+      <c r="A366" s="2">
+        <v>365</v>
+      </c>
+      <c r="B366" s="1">
         <v>22927.5</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A367" s="1">
-        <v>45657</v>
-      </c>
-      <c r="B367" s="2">
-        <v>49085.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>